<commit_message>
three studies left to analyze
</commit_message>
<xml_diff>
--- a/GroupPolarizationStatmod/data/CompletionProgressAndStatTest.xlsx
+++ b/GroupPolarizationStatmod/data/CompletionProgressAndStatTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mt/workspace/GroupPolarization/statmod/GroupPolarizationStatmod/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB986D21-CE4F-4640-AB11-358E9139FF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8600E63B-7C08-0342-B0F6-2993C72478FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{D3D3272A-2A6C-1948-91D2-7577447C3EB5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Tag</t>
   </si>
@@ -124,6 +124,21 @@
   </si>
   <si>
     <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Schkade2010</t>
+  </si>
+  <si>
+    <t>Myers1975</t>
+  </si>
+  <si>
+    <t>Moscovici1969</t>
+  </si>
+  <si>
+    <t>Krizan2007</t>
+  </si>
+  <si>
+    <t>Myers1970</t>
   </si>
 </sst>
 </file>
@@ -193,167 +208,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -391,6 +246,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -714,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3B8588-9009-3A49-A835-CEB2509C4ABD}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -791,29 +656,66 @@
         <v>13</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:B12">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+  <conditionalFormatting sqref="B3:B11">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="notEqual">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="notEqual">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C12">
-    <cfRule type="containsBlanks" dxfId="2" priority="2">
-      <formula>LEN(TRIM(C2))=0</formula>
-    </cfRule>
+  <conditionalFormatting sqref="C2:C11">
     <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(C2))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="0" priority="2">
+      <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finished data management and analysis required for generating simulated data
</commit_message>
<xml_diff>
--- a/GroupPolarizationStatmod/data/CompletionProgressAndStatTest.xlsx
+++ b/GroupPolarizationStatmod/data/CompletionProgressAndStatTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mt/workspace/GroupPolarization/statmod/GroupPolarizationStatmod/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8600E63B-7C08-0342-B0F6-2993C72478FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00BA11D-5F97-4944-98E8-F1796E03600C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{D3D3272A-2A6C-1948-91D2-7577447C3EB5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t>Tag</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>Close, needs a closer final look</t>
   </si>
   <si>
     <t>Burnstein1975</t>
@@ -139,6 +136,15 @@
   </si>
   <si>
     <t>Myers1970</t>
+  </si>
+  <si>
+    <t>Complete (N recorded for generating data)?</t>
+  </si>
+  <si>
+    <t>All results are BS? Paper uses ANOVA to compare shifts, but no significance testing of shifts</t>
+  </si>
+  <si>
+    <t>Several cases where it's not really group polarization: either polarity crosses neutral point or initial opinion is at neutral point; both of these seem to contradict the assumption of bias conservation.</t>
   </si>
 </sst>
 </file>
@@ -199,16 +205,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -579,20 +604,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3B8588-9009-3A49-A835-CEB2509C4ABD}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="3" width="33.83203125" customWidth="1"/>
-    <col min="4" max="4" width="56.1640625" customWidth="1"/>
+    <col min="2" max="4" width="33.83203125" customWidth="1"/>
+    <col min="5" max="5" width="56.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,25 +625,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -626,75 +659,116 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:B11">
+  <conditionalFormatting sqref="B3:C11">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="notEqual">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -702,20 +776,20 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+  <conditionalFormatting sqref="D2:D11">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="3">
+      <formula>LEN(TRIM(D2))&gt;0</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="2" priority="4">
+      <formula>LEN(TRIM(D2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="notEqual">
       <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C11">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(C2))&gt;0</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="0" priority="2">
-      <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>